<commit_message>
excel students with locations
</commit_message>
<xml_diff>
--- a/excel/students.xlsx
+++ b/excel/students.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cipleu\Documents\IULIA\SCOALA\facultate\Year 4 Semester 2\KBS\Lab\Project\University-Ontology\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8C1B423-C223-4576-9ED9-C20F2B699F7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DAD56A-8248-4B62-BADC-C1F07BC4754C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="218">
   <si>
     <t>FirstName</t>
   </si>
@@ -646,10 +646,34 @@
     <t>Address</t>
   </si>
   <si>
-    <t>Distance Baritiu</t>
-  </si>
-  <si>
-    <t>Distance Observator</t>
+    <t>101 Decebal Street</t>
+  </si>
+  <si>
+    <t>Distance Baritiu(km)</t>
+  </si>
+  <si>
+    <t>Distance Observator(km)</t>
+  </si>
+  <si>
+    <t>Distance Dorobantilor(km)</t>
+  </si>
+  <si>
+    <t>Distance Sport(km)</t>
+  </si>
+  <si>
+    <t>31 T. Mihali Street</t>
+  </si>
+  <si>
+    <t>Dorm 1F</t>
+  </si>
+  <si>
+    <t>Dorm Observator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13-11 Gheorghe Doja Street, Floresti</t>
+  </si>
+  <si>
+    <t>73-71 Iugoslaviei Street</t>
   </si>
 </sst>
 </file>
@@ -716,14 +740,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1026,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E110"/>
+  <dimension ref="A1:G110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C44" sqref="C44:G44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1066,7 @@
     <col min="2" max="2" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1049,882 +1077,2523 @@
         <v>207</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D2" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E2">
+        <v>4.3</v>
+      </c>
+      <c r="F2">
+        <v>2.6</v>
+      </c>
+      <c r="G2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D3">
+        <v>3.6</v>
+      </c>
+      <c r="E3">
+        <v>4.8</v>
+      </c>
+      <c r="F3">
+        <v>4.8</v>
+      </c>
+      <c r="G3">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>215</v>
+      </c>
+      <c r="D4">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E4">
+        <v>0.5</v>
+      </c>
+      <c r="F4">
+        <v>5.5</v>
+      </c>
+      <c r="G4">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D5">
+        <v>3.8</v>
+      </c>
+      <c r="E5">
+        <v>5</v>
+      </c>
+      <c r="F5">
+        <v>1.7</v>
+      </c>
+      <c r="G5">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D6">
+        <v>3.8</v>
+      </c>
+      <c r="E6">
+        <v>5</v>
+      </c>
+      <c r="F6">
+        <v>1.7</v>
+      </c>
+      <c r="G6">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>215</v>
+      </c>
+      <c r="D7">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E7">
+        <v>0.5</v>
+      </c>
+      <c r="F7">
+        <v>5.5</v>
+      </c>
+      <c r="G7">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>215</v>
+      </c>
+      <c r="D8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E8">
+        <v>0.5</v>
+      </c>
+      <c r="F8">
+        <v>5.5</v>
+      </c>
+      <c r="G8">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
       <c r="B9" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>215</v>
+      </c>
+      <c r="D9">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.5</v>
+      </c>
+      <c r="F9">
+        <v>5.5</v>
+      </c>
+      <c r="G9">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
       <c r="B10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>213</v>
+      </c>
+      <c r="D10">
+        <v>3.6</v>
+      </c>
+      <c r="E10">
+        <v>4.8</v>
+      </c>
+      <c r="F10">
+        <v>4.8</v>
+      </c>
+      <c r="G10">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
       <c r="B11" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>216</v>
+      </c>
+      <c r="D11">
+        <v>8.6</v>
+      </c>
+      <c r="E11">
+        <v>10.5</v>
+      </c>
+      <c r="F11">
+        <v>10.7</v>
+      </c>
+      <c r="G11">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>214</v>
+      </c>
+      <c r="D12">
+        <v>3.8</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>1.7</v>
+      </c>
+      <c r="G12">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>216</v>
+      </c>
+      <c r="D13">
+        <v>8.6</v>
+      </c>
+      <c r="E13">
+        <v>10.5</v>
+      </c>
+      <c r="F13">
+        <v>10.7</v>
+      </c>
+      <c r="G13">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E14">
+        <v>0.5</v>
+      </c>
+      <c r="F14">
+        <v>5.5</v>
+      </c>
+      <c r="G14">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15">
+        <v>3.4</v>
+      </c>
+      <c r="E15">
+        <v>4.5</v>
+      </c>
+      <c r="F15">
+        <v>1.7</v>
+      </c>
+      <c r="G15">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="B16" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>208</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E16">
+        <v>4.3</v>
+      </c>
+      <c r="F16">
+        <v>2.6</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>217</v>
+      </c>
+      <c r="D17">
+        <v>3.4</v>
+      </c>
+      <c r="E17">
+        <v>4.5</v>
+      </c>
+      <c r="F17">
+        <v>1.7</v>
+      </c>
+      <c r="G17">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
       <c r="B18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>216</v>
+      </c>
+      <c r="D18">
+        <v>8.6</v>
+      </c>
+      <c r="E18">
+        <v>10.5</v>
+      </c>
+      <c r="F18">
+        <v>10.7</v>
+      </c>
+      <c r="G18">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
       <c r="B19" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D19">
+        <v>3.8</v>
+      </c>
+      <c r="E19">
+        <v>5</v>
+      </c>
+      <c r="F19">
+        <v>1.7</v>
+      </c>
+      <c r="G19">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
       <c r="B20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>217</v>
+      </c>
+      <c r="D20">
+        <v>3.4</v>
+      </c>
+      <c r="E20">
+        <v>4.5</v>
+      </c>
+      <c r="F20">
+        <v>1.7</v>
+      </c>
+      <c r="G20">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>217</v>
+      </c>
+      <c r="D21">
+        <v>3.4</v>
+      </c>
+      <c r="E21">
+        <v>4.5</v>
+      </c>
+      <c r="F21">
+        <v>1.7</v>
+      </c>
+      <c r="G21">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>41</v>
       </c>
       <c r="B22" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>213</v>
+      </c>
+      <c r="D22">
+        <v>3.6</v>
+      </c>
+      <c r="E22">
+        <v>4.8</v>
+      </c>
+      <c r="F22">
+        <v>4.8</v>
+      </c>
+      <c r="G22">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>43</v>
       </c>
       <c r="B23" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>217</v>
+      </c>
+      <c r="D23">
+        <v>3.4</v>
+      </c>
+      <c r="E23">
+        <v>4.5</v>
+      </c>
+      <c r="F23">
+        <v>1.7</v>
+      </c>
+      <c r="G23">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>45</v>
       </c>
       <c r="B24" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>217</v>
+      </c>
+      <c r="D24">
+        <v>3.4</v>
+      </c>
+      <c r="E24">
+        <v>4.5</v>
+      </c>
+      <c r="F24">
+        <v>1.7</v>
+      </c>
+      <c r="G24">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>47</v>
       </c>
       <c r="B25" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>214</v>
+      </c>
+      <c r="D25">
+        <v>3.8</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="F25">
+        <v>1.7</v>
+      </c>
+      <c r="G25">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>49</v>
       </c>
       <c r="B26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>217</v>
+      </c>
+      <c r="D26">
+        <v>3.4</v>
+      </c>
+      <c r="E26">
+        <v>4.5</v>
+      </c>
+      <c r="F26">
+        <v>1.7</v>
+      </c>
+      <c r="G26">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>51</v>
       </c>
       <c r="B27" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D27">
+        <v>3.4</v>
+      </c>
+      <c r="E27">
+        <v>4.5</v>
+      </c>
+      <c r="F27">
+        <v>1.7</v>
+      </c>
+      <c r="G27">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>53</v>
       </c>
       <c r="B28" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>208</v>
+      </c>
+      <c r="D28" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E28">
+        <v>4.3</v>
+      </c>
+      <c r="F28">
+        <v>2.6</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>55</v>
       </c>
       <c r="B29" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>216</v>
+      </c>
+      <c r="D29">
+        <v>8.6</v>
+      </c>
+      <c r="E29">
+        <v>10.5</v>
+      </c>
+      <c r="F29">
+        <v>10.7</v>
+      </c>
+      <c r="G29">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>57</v>
       </c>
       <c r="B30" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>213</v>
+      </c>
+      <c r="D30">
+        <v>3.6</v>
+      </c>
+      <c r="E30">
+        <v>4.8</v>
+      </c>
+      <c r="F30">
+        <v>4.8</v>
+      </c>
+      <c r="G30">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>59</v>
       </c>
       <c r="B31" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>214</v>
+      </c>
+      <c r="D31">
+        <v>3.8</v>
+      </c>
+      <c r="E31">
+        <v>5</v>
+      </c>
+      <c r="F31">
+        <v>1.7</v>
+      </c>
+      <c r="G31">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>61</v>
       </c>
       <c r="B32" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>215</v>
+      </c>
+      <c r="D32">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E32">
+        <v>0.5</v>
+      </c>
+      <c r="F32">
+        <v>5.5</v>
+      </c>
+      <c r="G32">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>63</v>
       </c>
       <c r="B33" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>215</v>
+      </c>
+      <c r="D33">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E33">
+        <v>0.5</v>
+      </c>
+      <c r="F33">
+        <v>5.5</v>
+      </c>
+      <c r="G33">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>65</v>
       </c>
       <c r="B34" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>216</v>
+      </c>
+      <c r="D34">
+        <v>8.6</v>
+      </c>
+      <c r="E34">
+        <v>10.5</v>
+      </c>
+      <c r="F34">
+        <v>10.7</v>
+      </c>
+      <c r="G34">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>67</v>
       </c>
       <c r="B35" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>208</v>
+      </c>
+      <c r="D35" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E35">
+        <v>4.3</v>
+      </c>
+      <c r="F35">
+        <v>2.6</v>
+      </c>
+      <c r="G35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>69</v>
       </c>
       <c r="B36" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36" t="s">
+        <v>216</v>
+      </c>
+      <c r="D36">
+        <v>8.6</v>
+      </c>
+      <c r="E36">
+        <v>10.5</v>
+      </c>
+      <c r="F36">
+        <v>10.7</v>
+      </c>
+      <c r="G36">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>71</v>
       </c>
       <c r="B37" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37" t="s">
+        <v>214</v>
+      </c>
+      <c r="D37">
+        <v>3.8</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>1.7</v>
+      </c>
+      <c r="G37">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>73</v>
       </c>
       <c r="B38" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38" t="s">
+        <v>216</v>
+      </c>
+      <c r="D38">
+        <v>8.6</v>
+      </c>
+      <c r="E38">
+        <v>10.5</v>
+      </c>
+      <c r="F38">
+        <v>10.7</v>
+      </c>
+      <c r="G38">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>75</v>
       </c>
       <c r="B39" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>215</v>
+      </c>
+      <c r="D39">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E39">
+        <v>0.5</v>
+      </c>
+      <c r="F39">
+        <v>5.5</v>
+      </c>
+      <c r="G39">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>77</v>
       </c>
       <c r="B40" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40" t="s">
+        <v>216</v>
+      </c>
+      <c r="D40">
+        <v>8.6</v>
+      </c>
+      <c r="E40">
+        <v>10.5</v>
+      </c>
+      <c r="F40">
+        <v>10.7</v>
+      </c>
+      <c r="G40">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>79</v>
       </c>
       <c r="B41" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41" t="s">
+        <v>214</v>
+      </c>
+      <c r="D41">
+        <v>3.8</v>
+      </c>
+      <c r="E41">
+        <v>5</v>
+      </c>
+      <c r="F41">
+        <v>1.7</v>
+      </c>
+      <c r="G41">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>32</v>
       </c>
       <c r="B42" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42" t="s">
+        <v>216</v>
+      </c>
+      <c r="D42">
+        <v>8.6</v>
+      </c>
+      <c r="E42">
+        <v>10.5</v>
+      </c>
+      <c r="F42">
+        <v>10.7</v>
+      </c>
+      <c r="G42">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>82</v>
       </c>
       <c r="B43" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>208</v>
+      </c>
+      <c r="D43" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E43">
+        <v>4.3</v>
+      </c>
+      <c r="F43">
+        <v>2.6</v>
+      </c>
+      <c r="G43">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>84</v>
       </c>
       <c r="B44" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>216</v>
+      </c>
+      <c r="D44">
+        <v>8.6</v>
+      </c>
+      <c r="E44">
+        <v>10.5</v>
+      </c>
+      <c r="F44">
+        <v>10.7</v>
+      </c>
+      <c r="G44">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>86</v>
       </c>
       <c r="B45" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>214</v>
+      </c>
+      <c r="D45">
+        <v>3.8</v>
+      </c>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>1.7</v>
+      </c>
+      <c r="G45">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>88</v>
       </c>
       <c r="B46" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46" t="s">
+        <v>214</v>
+      </c>
+      <c r="D46">
+        <v>3.8</v>
+      </c>
+      <c r="E46">
+        <v>5</v>
+      </c>
+      <c r="F46">
+        <v>1.7</v>
+      </c>
+      <c r="G46">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>90</v>
       </c>
       <c r="B47" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>215</v>
+      </c>
+      <c r="D47">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E47">
+        <v>0.5</v>
+      </c>
+      <c r="F47">
+        <v>5.5</v>
+      </c>
+      <c r="G47">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>92</v>
       </c>
       <c r="B48" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>213</v>
+      </c>
+      <c r="D48">
+        <v>3.6</v>
+      </c>
+      <c r="E48">
+        <v>4.8</v>
+      </c>
+      <c r="F48">
+        <v>4.8</v>
+      </c>
+      <c r="G48">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>94</v>
       </c>
       <c r="B49" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49" t="s">
+        <v>216</v>
+      </c>
+      <c r="D49">
+        <v>8.6</v>
+      </c>
+      <c r="E49">
+        <v>10.5</v>
+      </c>
+      <c r="F49">
+        <v>10.7</v>
+      </c>
+      <c r="G49">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>96</v>
       </c>
       <c r="B50" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50" t="s">
+        <v>214</v>
+      </c>
+      <c r="D50">
+        <v>3.8</v>
+      </c>
+      <c r="E50">
+        <v>5</v>
+      </c>
+      <c r="F50">
+        <v>1.7</v>
+      </c>
+      <c r="G50">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>98</v>
       </c>
       <c r="B51" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>214</v>
+      </c>
+      <c r="D51">
+        <v>3.8</v>
+      </c>
+      <c r="E51">
+        <v>5</v>
+      </c>
+      <c r="F51">
+        <v>1.7</v>
+      </c>
+      <c r="G51">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>100</v>
       </c>
       <c r="B52" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52" t="s">
+        <v>215</v>
+      </c>
+      <c r="D52">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E52">
+        <v>0.5</v>
+      </c>
+      <c r="F52">
+        <v>5.5</v>
+      </c>
+      <c r="G52">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>102</v>
       </c>
       <c r="B53" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>216</v>
+      </c>
+      <c r="D53">
+        <v>8.6</v>
+      </c>
+      <c r="E53">
+        <v>10.5</v>
+      </c>
+      <c r="F53">
+        <v>10.7</v>
+      </c>
+      <c r="G53">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>104</v>
       </c>
       <c r="B54" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>213</v>
+      </c>
+      <c r="D54">
+        <v>3.6</v>
+      </c>
+      <c r="E54">
+        <v>4.8</v>
+      </c>
+      <c r="F54">
+        <v>4.8</v>
+      </c>
+      <c r="G54">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>106</v>
       </c>
       <c r="B55" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
+        <v>216</v>
+      </c>
+      <c r="D55">
+        <v>8.6</v>
+      </c>
+      <c r="E55">
+        <v>10.5</v>
+      </c>
+      <c r="F55">
+        <v>10.7</v>
+      </c>
+      <c r="G55">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>108</v>
       </c>
       <c r="B56" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56" t="s">
+        <v>215</v>
+      </c>
+      <c r="D56">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E56">
+        <v>0.5</v>
+      </c>
+      <c r="F56">
+        <v>5.5</v>
+      </c>
+      <c r="G56">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>109</v>
       </c>
       <c r="B57" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57" t="s">
+        <v>216</v>
+      </c>
+      <c r="D57">
+        <v>8.6</v>
+      </c>
+      <c r="E57">
+        <v>10.5</v>
+      </c>
+      <c r="F57">
+        <v>10.7</v>
+      </c>
+      <c r="G57">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>111</v>
       </c>
       <c r="B58" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>216</v>
+      </c>
+      <c r="D58">
+        <v>8.6</v>
+      </c>
+      <c r="E58">
+        <v>10.5</v>
+      </c>
+      <c r="F58">
+        <v>10.7</v>
+      </c>
+      <c r="G58">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>113</v>
       </c>
       <c r="B59" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59" t="s">
+        <v>216</v>
+      </c>
+      <c r="D59">
+        <v>8.6</v>
+      </c>
+      <c r="E59">
+        <v>10.5</v>
+      </c>
+      <c r="F59">
+        <v>10.7</v>
+      </c>
+      <c r="G59">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>115</v>
       </c>
       <c r="B60" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>208</v>
+      </c>
+      <c r="D60" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E60">
+        <v>4.3</v>
+      </c>
+      <c r="F60">
+        <v>2.6</v>
+      </c>
+      <c r="G60">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>117</v>
       </c>
       <c r="B61" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
+        <v>216</v>
+      </c>
+      <c r="D61">
+        <v>8.6</v>
+      </c>
+      <c r="E61">
+        <v>10.5</v>
+      </c>
+      <c r="F61">
+        <v>10.7</v>
+      </c>
+      <c r="G61">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>119</v>
       </c>
       <c r="B62" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62" t="s">
+        <v>215</v>
+      </c>
+      <c r="D62">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E62">
+        <v>0.5</v>
+      </c>
+      <c r="F62">
+        <v>5.5</v>
+      </c>
+      <c r="G62">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>121</v>
       </c>
       <c r="B63" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63" t="s">
+        <v>217</v>
+      </c>
+      <c r="D63">
+        <v>3.4</v>
+      </c>
+      <c r="E63">
+        <v>4.5</v>
+      </c>
+      <c r="F63">
+        <v>1.7</v>
+      </c>
+      <c r="G63">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>123</v>
       </c>
       <c r="B64" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64" t="s">
+        <v>214</v>
+      </c>
+      <c r="D64">
+        <v>3.8</v>
+      </c>
+      <c r="E64">
+        <v>5</v>
+      </c>
+      <c r="F64">
+        <v>1.7</v>
+      </c>
+      <c r="G64">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>125</v>
       </c>
       <c r="B65" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
+        <v>217</v>
+      </c>
+      <c r="D65">
+        <v>3.4</v>
+      </c>
+      <c r="E65">
+        <v>4.5</v>
+      </c>
+      <c r="F65">
+        <v>1.7</v>
+      </c>
+      <c r="G65">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>126</v>
       </c>
       <c r="B66" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
+        <v>216</v>
+      </c>
+      <c r="D66">
+        <v>8.6</v>
+      </c>
+      <c r="E66">
+        <v>10.5</v>
+      </c>
+      <c r="F66">
+        <v>10.7</v>
+      </c>
+      <c r="G66">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>128</v>
       </c>
       <c r="B67" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>217</v>
+      </c>
+      <c r="D67">
+        <v>3.4</v>
+      </c>
+      <c r="E67">
+        <v>4.5</v>
+      </c>
+      <c r="F67">
+        <v>1.7</v>
+      </c>
+      <c r="G67">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>130</v>
       </c>
       <c r="B68" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>216</v>
+      </c>
+      <c r="D68">
+        <v>8.6</v>
+      </c>
+      <c r="E68">
+        <v>10.5</v>
+      </c>
+      <c r="F68">
+        <v>10.7</v>
+      </c>
+      <c r="G68">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>132</v>
       </c>
       <c r="B69" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>208</v>
+      </c>
+      <c r="D69" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E69">
+        <v>4.3</v>
+      </c>
+      <c r="F69">
+        <v>2.6</v>
+      </c>
+      <c r="G69">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>63</v>
       </c>
       <c r="B70" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
+        <v>217</v>
+      </c>
+      <c r="D70">
+        <v>3.4</v>
+      </c>
+      <c r="E70">
+        <v>4.5</v>
+      </c>
+      <c r="F70">
+        <v>1.7</v>
+      </c>
+      <c r="G70">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>135</v>
       </c>
       <c r="B71" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
+        <v>216</v>
+      </c>
+      <c r="D71">
+        <v>8.6</v>
+      </c>
+      <c r="E71">
+        <v>10.5</v>
+      </c>
+      <c r="F71">
+        <v>10.7</v>
+      </c>
+      <c r="G71">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>137</v>
       </c>
       <c r="B72" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>208</v>
+      </c>
+      <c r="D72" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E72">
+        <v>4.3</v>
+      </c>
+      <c r="F72">
+        <v>2.6</v>
+      </c>
+      <c r="G72">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>139</v>
       </c>
       <c r="B73" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>216</v>
+      </c>
+      <c r="D73">
+        <v>8.6</v>
+      </c>
+      <c r="E73">
+        <v>10.5</v>
+      </c>
+      <c r="F73">
+        <v>10.7</v>
+      </c>
+      <c r="G73">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>141</v>
       </c>
       <c r="B74" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
+        <v>217</v>
+      </c>
+      <c r="D74">
+        <v>3.4</v>
+      </c>
+      <c r="E74">
+        <v>4.5</v>
+      </c>
+      <c r="F74">
+        <v>1.7</v>
+      </c>
+      <c r="G74">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>143</v>
       </c>
       <c r="B75" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
+        <v>213</v>
+      </c>
+      <c r="D75">
+        <v>3.6</v>
+      </c>
+      <c r="E75">
+        <v>4.8</v>
+      </c>
+      <c r="F75">
+        <v>4.8</v>
+      </c>
+      <c r="G75">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>145</v>
       </c>
       <c r="B76" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
+        <v>216</v>
+      </c>
+      <c r="D76">
+        <v>8.6</v>
+      </c>
+      <c r="E76">
+        <v>10.5</v>
+      </c>
+      <c r="F76">
+        <v>10.7</v>
+      </c>
+      <c r="G76">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>147</v>
       </c>
       <c r="B77" t="s">
         <v>148</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>215</v>
+      </c>
+      <c r="D77">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E77">
+        <v>0.5</v>
+      </c>
+      <c r="F77">
+        <v>5.5</v>
+      </c>
+      <c r="G77">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>149</v>
       </c>
       <c r="B78" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78" t="s">
+        <v>214</v>
+      </c>
+      <c r="D78">
+        <v>3.8</v>
+      </c>
+      <c r="E78">
+        <v>5</v>
+      </c>
+      <c r="F78">
+        <v>1.7</v>
+      </c>
+      <c r="G78">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>151</v>
       </c>
       <c r="B79" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>215</v>
+      </c>
+      <c r="D79">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E79">
+        <v>0.5</v>
+      </c>
+      <c r="F79">
+        <v>5.5</v>
+      </c>
+      <c r="G79">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>153</v>
       </c>
       <c r="B80" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
+        <v>208</v>
+      </c>
+      <c r="D80" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E80">
+        <v>4.3</v>
+      </c>
+      <c r="F80">
+        <v>2.6</v>
+      </c>
+      <c r="G80">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>155</v>
       </c>
       <c r="B81" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
+        <v>214</v>
+      </c>
+      <c r="D81">
+        <v>3.8</v>
+      </c>
+      <c r="E81">
+        <v>5</v>
+      </c>
+      <c r="F81">
+        <v>1.7</v>
+      </c>
+      <c r="G81">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>157</v>
       </c>
       <c r="B82" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82" t="s">
+        <v>215</v>
+      </c>
+      <c r="D82">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E82">
+        <v>0.5</v>
+      </c>
+      <c r="F82">
+        <v>5.5</v>
+      </c>
+      <c r="G82">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>158</v>
       </c>
       <c r="B83" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>215</v>
+      </c>
+      <c r="D83">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E83">
+        <v>0.5</v>
+      </c>
+      <c r="F83">
+        <v>5.5</v>
+      </c>
+      <c r="G83">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>159</v>
       </c>
       <c r="B84" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84" t="s">
+        <v>214</v>
+      </c>
+      <c r="D84">
+        <v>3.8</v>
+      </c>
+      <c r="E84">
+        <v>5</v>
+      </c>
+      <c r="F84">
+        <v>1.7</v>
+      </c>
+      <c r="G84">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>161</v>
       </c>
       <c r="B85" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>215</v>
+      </c>
+      <c r="D85">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E85">
+        <v>0.5</v>
+      </c>
+      <c r="F85">
+        <v>5.5</v>
+      </c>
+      <c r="G85">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>163</v>
       </c>
       <c r="B86" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>208</v>
+      </c>
+      <c r="D86" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E86">
+        <v>4.3</v>
+      </c>
+      <c r="F86">
+        <v>2.6</v>
+      </c>
+      <c r="G86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>165</v>
       </c>
       <c r="B87" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C87" t="s">
+        <v>213</v>
+      </c>
+      <c r="D87">
+        <v>3.6</v>
+      </c>
+      <c r="E87">
+        <v>4.8</v>
+      </c>
+      <c r="F87">
+        <v>4.8</v>
+      </c>
+      <c r="G87">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>88</v>
       </c>
       <c r="B88" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C88" t="s">
+        <v>214</v>
+      </c>
+      <c r="D88">
+        <v>3.8</v>
+      </c>
+      <c r="E88">
+        <v>5</v>
+      </c>
+      <c r="F88">
+        <v>1.7</v>
+      </c>
+      <c r="G88">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>168</v>
       </c>
       <c r="B89" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C89" t="s">
+        <v>213</v>
+      </c>
+      <c r="D89">
+        <v>3.6</v>
+      </c>
+      <c r="E89">
+        <v>4.8</v>
+      </c>
+      <c r="F89">
+        <v>4.8</v>
+      </c>
+      <c r="G89">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>170</v>
       </c>
       <c r="B90" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C90" t="s">
+        <v>214</v>
+      </c>
+      <c r="D90">
+        <v>3.8</v>
+      </c>
+      <c r="E90">
+        <v>5</v>
+      </c>
+      <c r="F90">
+        <v>1.7</v>
+      </c>
+      <c r="G90">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>126</v>
       </c>
       <c r="B91" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C91" t="s">
+        <v>214</v>
+      </c>
+      <c r="D91">
+        <v>3.8</v>
+      </c>
+      <c r="E91">
+        <v>5</v>
+      </c>
+      <c r="F91">
+        <v>1.7</v>
+      </c>
+      <c r="G91">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>117</v>
       </c>
       <c r="B92" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C92" t="s">
+        <v>215</v>
+      </c>
+      <c r="D92">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E92">
+        <v>0.5</v>
+      </c>
+      <c r="F92">
+        <v>5.5</v>
+      </c>
+      <c r="G92">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>174</v>
       </c>
       <c r="B93" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C93" t="s">
+        <v>213</v>
+      </c>
+      <c r="D93">
+        <v>3.6</v>
+      </c>
+      <c r="E93">
+        <v>4.8</v>
+      </c>
+      <c r="F93">
+        <v>4.8</v>
+      </c>
+      <c r="G93">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>176</v>
       </c>
       <c r="B94" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C94" t="s">
+        <v>213</v>
+      </c>
+      <c r="D94">
+        <v>3.6</v>
+      </c>
+      <c r="E94">
+        <v>4.8</v>
+      </c>
+      <c r="F94">
+        <v>4.8</v>
+      </c>
+      <c r="G94">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>178</v>
       </c>
       <c r="B95" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C95" t="s">
+        <v>217</v>
+      </c>
+      <c r="D95">
+        <v>3.4</v>
+      </c>
+      <c r="E95">
+        <v>4.5</v>
+      </c>
+      <c r="F95">
+        <v>1.7</v>
+      </c>
+      <c r="G95">
+        <v>5.7</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>180</v>
       </c>
       <c r="B96" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C96" t="s">
+        <v>213</v>
+      </c>
+      <c r="D96">
+        <v>3.6</v>
+      </c>
+      <c r="E96">
+        <v>4.8</v>
+      </c>
+      <c r="F96">
+        <v>4.8</v>
+      </c>
+      <c r="G96">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>182</v>
       </c>
       <c r="B97" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C97" t="s">
+        <v>214</v>
+      </c>
+      <c r="D97">
+        <v>3.8</v>
+      </c>
+      <c r="E97">
+        <v>5</v>
+      </c>
+      <c r="F97">
+        <v>1.7</v>
+      </c>
+      <c r="G97">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>184</v>
       </c>
       <c r="B98" t="s">
         <v>185</v>
       </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C98" t="s">
+        <v>208</v>
+      </c>
+      <c r="D98" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E98">
+        <v>4.3</v>
+      </c>
+      <c r="F98">
+        <v>2.6</v>
+      </c>
+      <c r="G98">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>186</v>
       </c>
       <c r="B99" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C99" t="s">
+        <v>214</v>
+      </c>
+      <c r="D99">
+        <v>3.8</v>
+      </c>
+      <c r="E99">
+        <v>5</v>
+      </c>
+      <c r="F99">
+        <v>1.7</v>
+      </c>
+      <c r="G99">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>65</v>
       </c>
       <c r="B100" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C100" t="s">
+        <v>213</v>
+      </c>
+      <c r="D100">
+        <v>3.6</v>
+      </c>
+      <c r="E100">
+        <v>4.8</v>
+      </c>
+      <c r="F100">
+        <v>4.8</v>
+      </c>
+      <c r="G100">
+        <v>9.6</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>189</v>
       </c>
       <c r="B101" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C101" t="s">
+        <v>215</v>
+      </c>
+      <c r="D101">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E101">
+        <v>0.5</v>
+      </c>
+      <c r="F101">
+        <v>5.5</v>
+      </c>
+      <c r="G101">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>191</v>
       </c>
       <c r="B102" t="s">
         <v>192</v>
       </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C102" t="s">
+        <v>208</v>
+      </c>
+      <c r="D102" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E102">
+        <v>4.3</v>
+      </c>
+      <c r="F102">
+        <v>2.6</v>
+      </c>
+      <c r="G102">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>193</v>
       </c>
       <c r="B103" t="s">
         <v>194</v>
       </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C103" t="s">
+        <v>208</v>
+      </c>
+      <c r="D103" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E103">
+        <v>4.3</v>
+      </c>
+      <c r="F103">
+        <v>2.6</v>
+      </c>
+      <c r="G103">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>195</v>
       </c>
       <c r="B104" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>214</v>
+      </c>
+      <c r="D104">
+        <v>3.8</v>
+      </c>
+      <c r="E104">
+        <v>5</v>
+      </c>
+      <c r="F104">
+        <v>1.7</v>
+      </c>
+      <c r="G104">
+        <v>6.4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>197</v>
       </c>
       <c r="B105" t="s">
         <v>198</v>
       </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>215</v>
+      </c>
+      <c r="D105">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E105">
+        <v>0.5</v>
+      </c>
+      <c r="F105">
+        <v>5.5</v>
+      </c>
+      <c r="G105">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>199</v>
       </c>
       <c r="B106" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C106" t="s">
+        <v>208</v>
+      </c>
+      <c r="D106" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E106">
+        <v>4.3</v>
+      </c>
+      <c r="F106">
+        <v>2.6</v>
+      </c>
+      <c r="G106">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>201</v>
       </c>
       <c r="B107" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C107" t="s">
+        <v>208</v>
+      </c>
+      <c r="D107" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E107">
+        <v>4.3</v>
+      </c>
+      <c r="F107">
+        <v>2.6</v>
+      </c>
+      <c r="G107">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>203</v>
       </c>
       <c r="B108" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C108" t="s">
+        <v>215</v>
+      </c>
+      <c r="D108">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E108">
+        <v>0.5</v>
+      </c>
+      <c r="F108">
+        <v>5.5</v>
+      </c>
+      <c r="G108">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>204</v>
       </c>
       <c r="B109" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C109" t="s">
+        <v>208</v>
+      </c>
+      <c r="D109" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="E109">
+        <v>4.3</v>
+      </c>
+      <c r="F109">
+        <v>2.6</v>
+      </c>
+      <c r="G109">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>205</v>
       </c>
       <c r="B110" t="s">
         <v>206</v>
+      </c>
+      <c r="C110" t="s">
+        <v>213</v>
+      </c>
+      <c r="D110">
+        <v>3.6</v>
+      </c>
+      <c r="E110">
+        <v>4.8</v>
+      </c>
+      <c r="F110">
+        <v>4.8</v>
+      </c>
+      <c r="G110">
+        <v>9.6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>